<commit_message>
minor updates to spreadsheets
</commit_message>
<xml_diff>
--- a/docs/1612019_SDG14_3_1_Metadata_submission_template_drop_QC.xlsx
+++ b/docs/1612019_SDG14_3_1_Metadata_submission_template_drop_QC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pieter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamb/oxy-work/OMD/OAPMetadataEditor/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F53ABD9-7EF6-B441-889C-11281B222C09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9942F83-6691-A846-A6DA-C7D2E5A1070F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="27340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="25000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -3570,7 +3570,7 @@
   <dimension ref="A1:X253"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A42" sqref="A41:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4570,7 +4570,7 @@
       <c r="Q39" s="151"/>
       <c r="R39" s="151"/>
     </row>
-    <row r="40" spans="1:18" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9">
         <v>38</v>
       </c>
@@ -4596,7 +4596,7 @@
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
     </row>
-    <row r="41" spans="1:18" s="12" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="9">
         <v>39</v>
       </c>
@@ -4622,7 +4622,7 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
     </row>
-    <row r="42" spans="1:18" s="12" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" s="12" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="13">
         <v>40</v>
       </c>
@@ -10399,7 +10399,7 @@
   <dimension ref="A1:P151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>